<commit_message>
Modified and updated all sleeper statements with setpage timeouts.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/NonPriceAgreementDetails.xlsx
+++ b/src/test/resources/datasheets/NonPriceAgreementDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="10995" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="AddNonPriceAgr_GlobalCatalog" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -48,25 +49,25 @@
     <t>REQUESTOR</t>
   </si>
   <si>
+    <t>iPhone_d_99_4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>CU-CUBIC</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>EA-EACH</t>
+  </si>
+  <si>
+    <t>Cell Phones</t>
+  </si>
+  <si>
     <t>XEEVA -MJ</t>
-  </si>
-  <si>
-    <t>Iphone</t>
-  </si>
-  <si>
-    <t>iPhone_d_99_4</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>CU-CUBIC</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>EA-EACH</t>
   </si>
 </sst>
 </file>
@@ -402,7 +403,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -441,28 +442,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>